<commit_message>
(refactor) add minor changes of different files for completeness
</commit_message>
<xml_diff>
--- a/Dokumentation.xlsx
+++ b/Dokumentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uwe Drauz\RProjects\bachelor_thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572A7B3E-9206-48B3-95A0-3D25049C494E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F41BBE7-DFD1-4C36-BEDC-E7A4339F9387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="13875" windowHeight="20116" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28065" yWindow="825" windowWidth="21600" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Modellvarianten" sheetId="1" r:id="rId1"/>
@@ -1161,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="F27" workbookViewId="0">
+      <selection activeCell="M34" sqref="M33:N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2408,7 +2408,13 @@
       <c r="K38" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="L38" s="37"/>
+      <c r="L38" s="37">
+        <v>57.66628</v>
+      </c>
+      <c r="M38" s="40">
+        <f>L38*(94/191)</f>
+        <v>28.380263455497385</v>
+      </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B39">
@@ -2448,7 +2454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F7965CB-45EB-4C41-8115-03F2FE0D0D87}">
   <dimension ref="B2:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>

</xml_diff>